<commit_message>
fix some error for Anova
</commit_message>
<xml_diff>
--- a/results/rest_tab.xlsx
+++ b/results/rest_tab.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>group</t>
   </si>
@@ -32,22 +32,28 @@
     <t>SE</t>
   </si>
   <si>
+    <t>significance</t>
+  </si>
+  <si>
     <t>pvalue</t>
   </si>
   <si>
-    <t>significance</t>
-  </si>
-  <si>
-    <t>setosa</t>
-  </si>
-  <si>
-    <t>versicolor</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>***</t>
+    <t>606</t>
+  </si>
+  <si>
+    <t>607</t>
+  </si>
+  <si>
+    <t>ZH11</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -129,25 +135,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>50.0</v>
+        <v>9.0</v>
       </c>
       <c r="C2" t="n">
-        <v>12.3</v>
+        <v>29.4</v>
       </c>
       <c r="D2" t="n">
-        <v>0.246</v>
+        <v>3.2667</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1054</v>
+        <v>0.1803</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0149</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
+        <v>0.0601</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="n">
+        <v>7.665750431301586E-14</v>
       </c>
     </row>
     <row r="3">
@@ -155,25 +161,51 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>50.0</v>
+        <v>9.0</v>
       </c>
       <c r="C3" t="n">
-        <v>66.3</v>
+        <v>11.7</v>
       </c>
       <c r="D3" t="n">
-        <v>1.326</v>
+        <v>1.3</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1978</v>
+        <v>0.2646</v>
       </c>
       <c r="F3" t="n">
-        <v>0.028</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
+        <v>0.0882</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="n">
+        <v>7.665750431301586E-14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.4444</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.3005</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.1002</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="n">
+        <v>7.665750431301586E-14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>